<commit_message>
Comiited on 23rd April by adding AgentSettingsWMC test and page
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/DownloadedFiles/SMS Response Template (1).xlsx
+++ b/ocms/src/test/resources/DownloadedFiles/SMS Response Template (1).xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="73">
   <si>
     <t xml:space="preserve">Text</t>
   </si>
@@ -163,67 +163,25 @@
     <t xml:space="preserve">24/10/2019 14:02:42</t>
   </si>
   <si>
-    <t xml:space="preserve">same</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vallue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1256</t>
-  </si>
-  <si>
-    <t xml:space="preserve">big</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3478</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qatetherfi\administrator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14/01/2020 12:54:02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMS Respon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMS Test2</t>
+    <t xml:space="preserve">Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Souce5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24/10/2019 14:00:41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestSM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMS Testing</t>
   </si>
   <si>
     <t xml:space="preserve">Template</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Updated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24/12/2019 15:58:11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Souce5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24/10/2019 14:00:41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TestSM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMS Testing</t>
   </si>
   <si>
     <t xml:space="preserve">18</t>
@@ -345,7 +303,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane state="frozen" ySplit="1" topLeftCell="A2"/>
@@ -591,226 +549,162 @@
     </row>
     <row r="8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
         <v>48</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
         <v>49</v>
       </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>50</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="F8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" t="s">
-        <v>55</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I9" t="s">
         <v>14</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I10" t="s">
         <v>14</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I11" t="s">
         <v>14</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" t="s">
+        <v>71</v>
+      </c>
+      <c r="I12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="B12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E12" t="s">
-        <v>75</v>
-      </c>
-      <c r="F12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G12" t="s">
-        <v>76</v>
-      </c>
-      <c r="H12" t="s">
-        <v>75</v>
-      </c>
-      <c r="I12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F13" t="s">
-        <v>81</v>
-      </c>
-      <c r="G13" t="s">
-        <v>81</v>
-      </c>
-      <c r="H13" t="s">
-        <v>81</v>
-      </c>
-      <c r="I13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>83</v>
-      </c>
-      <c r="B14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" t="s">
-        <v>85</v>
-      </c>
-      <c r="F14" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" t="s">
-        <v>83</v>
-      </c>
-      <c r="H14" t="s">
-        <v>85</v>
-      </c>
-      <c r="I14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>